<commit_message>
Reading HTML Form Data with Servlets
</commit_message>
<xml_diff>
--- a/me_docs/8.Servlet-Fundamentals.xlsx
+++ b/me_docs/8.Servlet-Fundamentals.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B0677B-9D9F-4FBE-8D36-1452EDDAE212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0071BCF-73A7-4FCC-AB1B-0DA31CB6F891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create servletdemo project" sheetId="1" r:id="rId1"/>
     <sheet name="Create HelloWorldServle Servlet" sheetId="2" r:id="rId2"/>
+    <sheet name="Reading HTML Form Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Create servletdemo project</t>
   </si>
@@ -43,7 +44,22 @@
     <t>Access URL to test: http://localhost:8080/servletdemo/HelloWorldServlet</t>
   </si>
   <si>
-    <t>HelloWorldServlet</t>
+    <t>Reading HTML Form Data with Servlets</t>
+  </si>
+  <si>
+    <t>Create student-form.html</t>
+  </si>
+  <si>
+    <t>Create HelloWorldServlet</t>
+  </si>
+  <si>
+    <t>Create StudentServlet Servlet</t>
+  </si>
+  <si>
+    <t>Access browser to test</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/servletdemo/student-form.html</t>
   </si>
 </sst>
 </file>
@@ -79,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,6 +862,495 @@
         <a:xfrm>
           <a:off x="609600" y="47434500"/>
           <a:ext cx="4914286" cy="2057143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>37257</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>113738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2562681-759B-43FE-B052-80ACA500535C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="762000"/>
+          <a:ext cx="6742857" cy="4495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>599467</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>170738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A67EDA22-489C-4324-960B-AC399415E447}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5524500"/>
+          <a:ext cx="4866667" cy="5695238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>494400</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>113786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBEE4634-CB80-433C-944A-B7727F387F6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="11430000"/>
+          <a:ext cx="7200000" cy="4114286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>65828</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>46976</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D5843D1-9DCB-474F-90FD-3E7AA722209A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="16002000"/>
+          <a:ext cx="6771428" cy="5190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>570895</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>171000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{763A248C-88D9-4484-99D0-9D6DC0420304}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="21336000"/>
+          <a:ext cx="4838095" cy="3600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>570057</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>170690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A536D32C-339E-421F-991E-18841568B4DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="25146000"/>
+          <a:ext cx="11542857" cy="6076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>560533</xdr:colOff>
+      <xdr:row>198</xdr:row>
+      <xdr:rowOff>46881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BAF77AD-B00D-4982-BA73-8AD6557B1FBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="31813500"/>
+          <a:ext cx="11533333" cy="5952381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>255695</xdr:colOff>
+      <xdr:row>229</xdr:row>
+      <xdr:rowOff>8881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF691930-181E-4186-87B9-B336ED523C54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="40957500"/>
+          <a:ext cx="11838095" cy="5152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>275581</xdr:colOff>
+      <xdr:row>263</xdr:row>
+      <xdr:rowOff>142071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AF3B902-469F-42AC-B7BB-8FBADD65F355}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="43815000"/>
+          <a:ext cx="5152381" cy="6428571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>267</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>37486</xdr:colOff>
+      <xdr:row>277</xdr:row>
+      <xdr:rowOff>133095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71C2D1B1-5172-48BD-AC12-3DCFFCCC1CDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="50863500"/>
+          <a:ext cx="4914286" cy="2038095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>278</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>46781</xdr:colOff>
+      <xdr:row>286</xdr:row>
+      <xdr:rowOff>133143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D753D326-FE5A-4591-98CE-D7EADA4551D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="52959000"/>
+          <a:ext cx="6752381" cy="1657143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1147,15 +1653,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02C65FA-3DB2-4305-8ED1-E52EF82748A4}">
   <dimension ref="A2:A249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="N225" sqref="N225"/>
+    <sheetView topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="J263" sqref="J263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
@@ -1177,4 +1683,55 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E946FFB-D605-417A-9D6F-E15662C9158C}">
+  <dimension ref="A2:E267"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
+      <selection activeCell="E289" sqref="E289"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B267" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>